<commit_message>
Navbar is translatable now!!!
</commit_message>
<xml_diff>
--- a/translation.xlsx
+++ b/translation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\P_Faunistica\fau_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9920CF0F-F739-44CB-B600-47B6A9498F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E876611-88FA-44F1-973D-FB50724D15FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{02C04964-5ED9-4063-A933-2BC0206A63F1}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{02C04964-5ED9-4063-A933-2BC0206A63F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
   <si>
     <t>block</t>
   </si>
@@ -49,6 +49,153 @@
   </si>
   <si>
     <t>curretnt_language</t>
+  </si>
+  <si>
+    <t>page1</t>
+  </si>
+  <si>
+    <t>Страница 1</t>
+  </si>
+  <si>
+    <t>Page one</t>
+  </si>
+  <si>
+    <t>Page two</t>
+  </si>
+  <si>
+    <t>Страница 2</t>
+  </si>
+  <si>
+    <t>page2</t>
+  </si>
+  <si>
+    <t>nv</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>Главная</t>
+  </si>
+  <si>
+    <t>Start page</t>
+  </si>
+  <si>
+    <t>Статистика</t>
+  </si>
+  <si>
+    <t>Участвовать!</t>
+  </si>
+  <si>
+    <t>Participate!</t>
+  </si>
+  <si>
+    <t>Statistics</t>
+  </si>
+  <si>
+    <t>О проекте</t>
+  </si>
+  <si>
+    <t>About</t>
+  </si>
+  <si>
+    <t>Для волонтеров</t>
+  </si>
+  <si>
+    <t>Польза для науки</t>
+  </si>
+  <si>
+    <t>Польза для вас</t>
+  </si>
+  <si>
+    <t>Как нам помочь</t>
+  </si>
+  <si>
+    <t>Наш волонтерский проект</t>
+  </si>
+  <si>
+    <t>Для специалистов</t>
+  </si>
+  <si>
+    <t>Сотрудничество</t>
+  </si>
+  <si>
+    <t>Наше веб-приложение</t>
+  </si>
+  <si>
+    <t>Наш научный проект</t>
+  </si>
+  <si>
+    <t>Наша команда</t>
+  </si>
+  <si>
+    <t>Our team</t>
+  </si>
+  <si>
+    <t>Profit for science</t>
+  </si>
+  <si>
+    <t>Profit for you</t>
+  </si>
+  <si>
+    <t>How to help</t>
+  </si>
+  <si>
+    <t>For volunteers</t>
+  </si>
+  <si>
+    <t>Our voluntary project</t>
+  </si>
+  <si>
+    <t>For scientists</t>
+  </si>
+  <si>
+    <t>Cooperation</t>
+  </si>
+  <si>
+    <t>Our scientific project</t>
+  </si>
+  <si>
+    <t>participate</t>
+  </si>
+  <si>
+    <t>statistics</t>
+  </si>
+  <si>
+    <t>about</t>
+  </si>
+  <si>
+    <t>team</t>
+  </si>
+  <si>
+    <t>for_volunteers</t>
+  </si>
+  <si>
+    <t>profit_science</t>
+  </si>
+  <si>
+    <t>profit_personal</t>
+  </si>
+  <si>
+    <t>howtohelp</t>
+  </si>
+  <si>
+    <t>voluntary_project</t>
+  </si>
+  <si>
+    <t>for_scientists</t>
+  </si>
+  <si>
+    <t>cooperation</t>
+  </si>
+  <si>
+    <t>web_app</t>
+  </si>
+  <si>
+    <t>Our web-application</t>
+  </si>
+  <si>
+    <t>scientific_project</t>
   </si>
 </sst>
 </file>
@@ -401,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF9DD755-9DD9-4377-9219-883035337107}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -441,6 +588,230 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
(completely) new version (stable)
</commit_message>
<xml_diff>
--- a/translation.xlsx
+++ b/translation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\P_Faunistica\fau_test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\P_Faunistica\fau_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239E394F-83D6-42C3-9913-5816116D397B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A9F075-E521-4B02-8701-06B4D70D58D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{02C04964-5ED9-4063-A933-2BC0206A63F1}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{02C04964-5ED9-4063-A933-2BC0206A63F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -414,9 +414,6 @@
     <t>Точное расположение</t>
   </si>
   <si>
-    <t>Прочие примечания</t>
-  </si>
-  <si>
     <t>Georeference remarks</t>
   </si>
   <si>
@@ -441,9 +438,6 @@
     <t>Зафиксировать информацию в этом блоке</t>
   </si>
   <si>
-    <t>Данные пробы</t>
-  </si>
-  <si>
     <t>Дата</t>
   </si>
   <si>
@@ -453,9 +447,6 @@
     <t>Выборочное усилие</t>
   </si>
   <si>
-    <t>Комментарии</t>
-  </si>
-  <si>
     <t>Sampling event</t>
   </si>
   <si>
@@ -666,7 +657,16 @@
     <t>&lt;tt&gt;Вход выполнен: &lt;span style="color: blacl; background-color: lime;"&gt; ДА ✔ &lt;/span&gt;&lt;br&gt;Возможность записи: &lt;span style="color: black; background-color: lime;"&gt; ДА ✔ &lt;/span&gt;&lt;/tt&gt;</t>
   </si>
   <si>
-    <t>Перед вводом данных необходимо авторизоваться. &lt;br&gt;Получить пароль можно у</t>
+    <t>Первым делом необходимо авторизоваться. &lt;br&gt;Получить пароль можно у</t>
+  </si>
+  <si>
+    <t>Сбор материала</t>
+  </si>
+  <si>
+    <t>Примечания к расположению</t>
+  </si>
+  <si>
+    <t>Примечания к сбору материала</t>
   </si>
 </sst>
 </file>
@@ -1036,8 +1036,8 @@
   <dimension ref="A1:D77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C38" sqref="C38"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1083,7 +1083,7 @@
         <v>94</v>
       </c>
       <c r="C3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D3" t="s">
         <v>97</v>
@@ -1108,13 +1108,13 @@
         <v>93</v>
       </c>
       <c r="B5" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D5" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1122,13 +1122,13 @@
         <v>93</v>
       </c>
       <c r="B6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C6" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D6" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1559,10 +1559,10 @@
         <v>109</v>
       </c>
       <c r="C37" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D37" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1587,10 +1587,10 @@
         <v>110</v>
       </c>
       <c r="C39" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D39" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1626,13 +1626,13 @@
         <v>83</v>
       </c>
       <c r="B42" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C42" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D42" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -1640,13 +1640,13 @@
         <v>83</v>
       </c>
       <c r="B43" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C43" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D43" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -1674,7 +1674,7 @@
         <v>128</v>
       </c>
       <c r="D45" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -1685,10 +1685,10 @@
         <v>124</v>
       </c>
       <c r="C46" t="s">
+        <v>212</v>
+      </c>
+      <c r="D46" t="s">
         <v>129</v>
-      </c>
-      <c r="D46" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -1699,10 +1699,10 @@
         <v>125</v>
       </c>
       <c r="C47" t="s">
+        <v>131</v>
+      </c>
+      <c r="D47" t="s">
         <v>132</v>
-      </c>
-      <c r="D47" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -1710,13 +1710,13 @@
         <v>83</v>
       </c>
       <c r="B48" t="s">
+        <v>133</v>
+      </c>
+      <c r="C48" t="s">
         <v>134</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>135</v>
-      </c>
-      <c r="D48" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -1724,13 +1724,13 @@
         <v>83</v>
       </c>
       <c r="B49" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C49" t="s">
-        <v>138</v>
+        <v>211</v>
       </c>
       <c r="D49" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -1738,13 +1738,13 @@
         <v>83</v>
       </c>
       <c r="B50" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C50" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D50" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1752,13 +1752,13 @@
         <v>83</v>
       </c>
       <c r="B51" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C51" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D51" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -1766,13 +1766,13 @@
         <v>83</v>
       </c>
       <c r="B52" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C52" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D52" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -1780,13 +1780,13 @@
         <v>83</v>
       </c>
       <c r="B53" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C53" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D53" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -1794,13 +1794,13 @@
         <v>83</v>
       </c>
       <c r="B54" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C54" t="s">
-        <v>142</v>
+        <v>213</v>
       </c>
       <c r="D54" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -1808,13 +1808,13 @@
         <v>83</v>
       </c>
       <c r="B55" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C55" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D55" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -1822,13 +1822,13 @@
         <v>83</v>
       </c>
       <c r="B56" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C56" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D56" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -1836,13 +1836,13 @@
         <v>83</v>
       </c>
       <c r="B57" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C57" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D57" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -1850,13 +1850,13 @@
         <v>83</v>
       </c>
       <c r="B58" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C58" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D58" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -1864,13 +1864,13 @@
         <v>83</v>
       </c>
       <c r="B59" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C59" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D59" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -1878,13 +1878,13 @@
         <v>83</v>
       </c>
       <c r="B60" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C60" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D60" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -1892,13 +1892,13 @@
         <v>83</v>
       </c>
       <c r="B61" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C61" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D61" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -1906,13 +1906,13 @@
         <v>83</v>
       </c>
       <c r="B62" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C62" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D62" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -1920,13 +1920,13 @@
         <v>83</v>
       </c>
       <c r="B63" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C63" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D63" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -1934,13 +1934,13 @@
         <v>83</v>
       </c>
       <c r="B64" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C64" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D64" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -1948,13 +1948,13 @@
         <v>83</v>
       </c>
       <c r="B65" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C65" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D65" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -1962,13 +1962,13 @@
         <v>83</v>
       </c>
       <c r="B66" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C66" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D66" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -1976,13 +1976,13 @@
         <v>83</v>
       </c>
       <c r="B67" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C67" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D67" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -1990,13 +1990,13 @@
         <v>83</v>
       </c>
       <c r="B68" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C68" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D68" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -2004,13 +2004,13 @@
         <v>83</v>
       </c>
       <c r="B69" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C69" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D69" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>